<commit_message>
Actualizar ESTATUS.xlsx con datos de la semana
</commit_message>
<xml_diff>
--- a/ESTATUS.xlsx
+++ b/ESTATUS.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\ESTATUS_ENVIO_CONDCUTORES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B70C297A-37FD-47E0-A505-701113378644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698C70B5-885D-4A9C-972F-C283D20B6EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{381F552A-E5BE-4D47-BD36-97BB1A35D9B1}"/>
   </bookViews>
@@ -36,12 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
   <si>
     <t>MOVIL</t>
   </si>
   <si>
     <t>servicios</t>
+  </si>
+  <si>
+    <t>Flota</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Aeropuerto</t>
+  </si>
+  <si>
+    <t>Plaza</t>
+  </si>
+  <si>
+    <t>Aerolinea</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
   </si>
 </sst>
 </file>
@@ -83,7 +101,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -97,15 +119,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{987D297A-F2E9-4BC9-B2CF-AFDDAE57A151}" name="Tabla1" displayName="Tabla1" ref="A1:B22" totalsRowShown="0">
-  <autoFilter ref="A1:B22" xr:uid="{987D297A-F2E9-4BC9-B2CF-AFDDAE57A151}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FC930282-61FF-4CEF-8A25-CF9080D0CF6E}" name="MOVIL">
-      <calculatedColumnFormula>A1+1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{F5CE56E6-D47E-487D-B16E-E12E3D792A21}" name="servicios">
-      <calculatedColumnFormula>RANDBETWEEN(12,35)</calculatedColumnFormula>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{987D297A-F2E9-4BC9-B2CF-AFDDAE57A151}" name="Tabla1" displayName="Tabla1" ref="A1:D22" totalsRowShown="0">
+  <autoFilter ref="A1:D22" xr:uid="{987D297A-F2E9-4BC9-B2CF-AFDDAE57A151}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FC930282-61FF-4CEF-8A25-CF9080D0CF6E}" name="MOVIL"/>
+    <tableColumn id="2" xr3:uid="{F5CE56E6-D47E-487D-B16E-E12E3D792A21}" name="servicios"/>
+    <tableColumn id="3" xr3:uid="{5B807A11-D74E-44AA-AAE9-B2FD9E16676D}" name="Flota"/>
+    <tableColumn id="4" xr3:uid="{392B218F-A076-47DD-912E-FF617FF85A43}" name="Meta" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,229 +448,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA107D9-97F4-44C6-B039-6F1CAE12D6EA}">
-  <dimension ref="A1:B22"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>8574</v>
       </c>
       <c r="B2">
-        <f ca="1">RANDBETWEEN(12,35)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>A2+1</f>
+        <v>8658</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7403</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8055</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>7135</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9123</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8760</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7568</v>
+      </c>
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7519</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8852</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8902</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8257</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7716</v>
+      </c>
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B22" ca="1" si="0">RANDBETWEEN(12,35)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" ref="A4:A22" si="1">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="1"/>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>8640</v>
+      </c>
+      <c r="B15">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6875</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="1"/>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>7350</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>9084</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>8811</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>8665</v>
+      </c>
+      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <f t="shared" ca="1" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="1"/>
+      <c r="D20">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f t="shared" ca="1" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>8752</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>8675</v>
+      </c>
+      <c r="B22">
         <v>12</v>
       </c>
-      <c r="B13">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <f t="shared" ca="1" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <f t="shared" ca="1" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>